<commit_message>
update class projects, add DAGs
</commit_message>
<xml_diff>
--- a/Projects/Federal Reserve Data/SUR2005-12-31-2008-09-30.xlsx
+++ b/Projects/Federal Reserve Data/SUR2005-12-31-2008-09-30.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>CA_LF</t>
+  </si>
+  <si>
+    <t>FFR_LF</t>
+  </si>
+  <si>
     <t>LF_CA</t>
   </si>
   <si>
     <t>LF_FFR</t>
-  </si>
-  <si>
-    <t>FFR_LF</t>
-  </si>
-  <si>
-    <t>CA_LF</t>
   </si>
   <si>
     <t>params</t>
@@ -414,16 +414,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.1382174556653222</v>
+        <v>0.9168477780017975</v>
       </c>
       <c r="C2">
-        <v>0.6148321271736873</v>
+        <v>1.406551190655028</v>
       </c>
       <c r="D2">
-        <v>1.406551190655027</v>
+        <v>0.1382174556653223</v>
       </c>
       <c r="E2">
-        <v>0.9168477780017975</v>
+        <v>0.6148321271736868</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -431,16 +431,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.81484669514731E-08</v>
+        <v>1.486500189606943E-06</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
+        <v>1.81484669514731E-08</v>
+      </c>
+      <c r="E3">
         <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1.486500189606943E-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>